<commit_message>
updated commonwealth flag focus icon
</commit_message>
<xml_diff>
--- a/BiceE Documentation/ENG Historical Plan.xlsx
+++ b/BiceE Documentation/ENG Historical Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Rankin\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-Expanded\BiceE Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26416361-D76A-482B-BE2F-1D80C494F551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A960C-91F1-4418-A710-5D0FC11D343A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{4CEBE7C9-E6FE-4393-BB13-E322055FE4E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{4CEBE7C9-E6FE-4393-BB13-E322055FE4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,214 +158,217 @@
     <t>ENG_Limited_Liability</t>
   </si>
   <si>
+    <t>ENG_prepare_for_the_inevitable</t>
+  </si>
+  <si>
+    <t>uk_protect_suez</t>
+  </si>
+  <si>
+    <t>uk_malta_focus</t>
+  </si>
+  <si>
+    <t>air_defense_focus</t>
+  </si>
+  <si>
+    <t>ENG_artillery_focus</t>
+  </si>
+  <si>
+    <t>ENG_continental_warfare</t>
+  </si>
+  <si>
+    <t>hongkong_focus</t>
+  </si>
+  <si>
+    <t>hk_landward_forts_focus</t>
+  </si>
+  <si>
+    <t>sp_landward_forts_focus</t>
+  </si>
+  <si>
+    <t>peninsular_focus</t>
+  </si>
+  <si>
+    <t>ENG_home_defence</t>
+  </si>
+  <si>
+    <t>uk_commonwealth_focus</t>
+  </si>
+  <si>
+    <t>uk_canada_focus</t>
+  </si>
+  <si>
+    <t>uk_india_focus</t>
+  </si>
+  <si>
+    <t>uk_australia_focus</t>
+  </si>
+  <si>
+    <t>uk_new_zealand_focus</t>
+  </si>
+  <si>
+    <t>uk_commonwealth_knowledge</t>
+  </si>
+  <si>
+    <t>ENG_upgrade_old_BBs</t>
+  </si>
+  <si>
+    <t>ENG_press_censorship</t>
+  </si>
+  <si>
+    <t>ENG_military_training_act</t>
+  </si>
+  <si>
+    <t>ENG_peace_has_failed</t>
+  </si>
+  <si>
+    <t>ENG_EPA</t>
+  </si>
+  <si>
+    <t>ENG_BEF</t>
+  </si>
+  <si>
+    <t>ENG_Port_Garrisons</t>
+  </si>
+  <si>
+    <t>ENG_seek_help_abroad</t>
+  </si>
+  <si>
+    <t>crypto_bomb_focus</t>
+  </si>
+  <si>
+    <t>ENG_home_front</t>
+  </si>
+  <si>
+    <t>ENG_issue_gasmasks</t>
+  </si>
+  <si>
+    <t>ENG_industrial_programme_focus2</t>
+  </si>
+  <si>
+    <t>ENG_national_registration_act</t>
+  </si>
+  <si>
+    <t>radar_focus</t>
+  </si>
+  <si>
+    <t>royal_ordinance_focus</t>
+  </si>
+  <si>
+    <t>ENG_ration_petrol</t>
+  </si>
+  <si>
+    <t>tizard_mission_focus</t>
+  </si>
+  <si>
+    <t>ENG_beaverbrook</t>
+  </si>
+  <si>
+    <t>ENG_chiefs_of_staff_committee</t>
+  </si>
+  <si>
+    <t>uk_small_arms_focus</t>
+  </si>
+  <si>
+    <t>ENG_seek_help_from_usa</t>
+  </si>
+  <si>
+    <t>ENG_HomeGuard</t>
+  </si>
+  <si>
+    <t>ENG_time_is_now</t>
+  </si>
+  <si>
+    <t>ENG_GHQ_Line</t>
+  </si>
+  <si>
+    <t>ENG_purchase_usa_planes</t>
+  </si>
+  <si>
+    <t>ENG_raf_ace_program</t>
+  </si>
+  <si>
+    <t>uk_convoy_focus</t>
+  </si>
+  <si>
+    <t>ENG_skies</t>
+  </si>
+  <si>
+    <t>ENG_AA</t>
+  </si>
+  <si>
+    <t>uk_anglo_soviet_occupation</t>
+  </si>
+  <si>
+    <t>ENG_inchindown_tanks</t>
+  </si>
+  <si>
+    <t>ENG_anti_submarine_training_school</t>
+  </si>
+  <si>
+    <t>ENG_radar_networks</t>
+  </si>
+  <si>
+    <t>ENG_NSA</t>
+  </si>
+  <si>
+    <t>ENG_special_air_service</t>
+  </si>
+  <si>
+    <t>ENG_defend_the_commonwealth</t>
+  </si>
+  <si>
+    <t>ENG_anzac_force</t>
+  </si>
+  <si>
+    <t>ENG_defend_ast</t>
+  </si>
+  <si>
+    <t>ENG_heavy_aircraft_research</t>
+  </si>
+  <si>
+    <t>ENG_peoples_war</t>
+  </si>
+  <si>
+    <t>ENG_ration_civ_clothing</t>
+  </si>
+  <si>
+    <t>ENG_motorized_focus</t>
+  </si>
+  <si>
+    <t>ENG_tank_focus</t>
+  </si>
+  <si>
+    <t>ENG_cruiser_tanks</t>
+  </si>
+  <si>
+    <t>ENG_bouncing_bomb</t>
+  </si>
+  <si>
+    <t>ENG_support_france</t>
+  </si>
+  <si>
     <t>ENG_deploy_kgv_BBs</t>
   </si>
   <si>
-    <t>ENG_prepare_for_the_inevitable</t>
-  </si>
-  <si>
-    <t>uk_protect_suez</t>
-  </si>
-  <si>
-    <t>uk_malta_focus</t>
-  </si>
-  <si>
-    <t>air_defense_focus</t>
-  </si>
-  <si>
     <t>ENG_deploy_illustrious_class</t>
   </si>
   <si>
-    <t>ENG_artillery_focus</t>
-  </si>
-  <si>
-    <t>ENG_continental_warfare</t>
-  </si>
-  <si>
-    <t>hongkong_focus</t>
-  </si>
-  <si>
-    <t>hk_landward_forts_focus</t>
-  </si>
-  <si>
-    <t>sp_landward_forts_focus</t>
-  </si>
-  <si>
-    <t>peninsular_focus</t>
+    <t>ENG_Blockade_Germany</t>
   </si>
   <si>
     <t>ENG_deploy_hms_indomitable</t>
   </si>
   <si>
     <t>ENG_deploy_duke_of_york</t>
-  </si>
-  <si>
-    <t>ENG_home_defence</t>
-  </si>
-  <si>
-    <t>uk_commonwealth_focus</t>
-  </si>
-  <si>
-    <t>uk_canada_focus</t>
-  </si>
-  <si>
-    <t>uk_india_focus</t>
-  </si>
-  <si>
-    <t>uk_australia_focus</t>
-  </si>
-  <si>
-    <t>uk_new_zealand_focus</t>
-  </si>
-  <si>
-    <t>uk_commonwealth_knowledge</t>
-  </si>
-  <si>
-    <t>ENG_upgrade_old_BBs</t>
-  </si>
-  <si>
-    <t>ENG_press_censorship</t>
-  </si>
-  <si>
-    <t>ENG_military_training_act</t>
-  </si>
-  <si>
-    <t>ENG_peace_has_failed</t>
-  </si>
-  <si>
-    <t>ENG_Blockade_Germany</t>
-  </si>
-  <si>
-    <t>ENG_EPA</t>
-  </si>
-  <si>
-    <t>ENG_BEF</t>
-  </si>
-  <si>
-    <t>ENG_Port_Garrisons</t>
-  </si>
-  <si>
-    <t>ENG_seek_help_abroad</t>
-  </si>
-  <si>
-    <t>crypto_bomb_focus</t>
-  </si>
-  <si>
-    <t>ENG_home_front</t>
-  </si>
-  <si>
-    <t>ENG_issue_gasmasks</t>
-  </si>
-  <si>
-    <t>ENG_industrial_programme_focus2</t>
-  </si>
-  <si>
-    <t>ENG_national_registration_act</t>
-  </si>
-  <si>
-    <t>radar_focus</t>
-  </si>
-  <si>
-    <t>royal_ordinance_focus</t>
-  </si>
-  <si>
-    <t>ENG_ration_petrol</t>
-  </si>
-  <si>
-    <t>tizard_mission_focus</t>
-  </si>
-  <si>
-    <t>ENG_beaverbrook</t>
-  </si>
-  <si>
-    <t>ENG_chiefs_of_staff_committee</t>
-  </si>
-  <si>
-    <t>uk_small_arms_focus</t>
-  </si>
-  <si>
-    <t>ENG_seek_help_from_usa</t>
-  </si>
-  <si>
-    <t>ENG_HomeGuard</t>
-  </si>
-  <si>
-    <t>ENG_time_is_now</t>
-  </si>
-  <si>
-    <t>ENG_GHQ_Line</t>
-  </si>
-  <si>
-    <t>ENG_purchase_usa_planes</t>
-  </si>
-  <si>
-    <t>ENG_raf_ace_program</t>
-  </si>
-  <si>
-    <t>uk_convoy_focus</t>
-  </si>
-  <si>
-    <t>ENG_skies</t>
-  </si>
-  <si>
-    <t>ENG_AA</t>
-  </si>
-  <si>
-    <t>uk_anglo_soviet_occupation</t>
-  </si>
-  <si>
-    <t>ENG_inchindown_tanks</t>
-  </si>
-  <si>
-    <t>ENG_anti_submarine_training_school</t>
-  </si>
-  <si>
-    <t>ENG_radar_networks</t>
-  </si>
-  <si>
-    <t>ENG_NSA</t>
-  </si>
-  <si>
-    <t>ENG_special_air_service</t>
-  </si>
-  <si>
-    <t>ENG_defend_the_commonwealth</t>
-  </si>
-  <si>
-    <t>ENG_anzac_force</t>
-  </si>
-  <si>
-    <t>ENG_defend_ast</t>
-  </si>
-  <si>
-    <t>ENG_heavy_aircraft_research</t>
-  </si>
-  <si>
-    <t>ENG_peoples_war</t>
-  </si>
-  <si>
-    <t>ENG_ration_civ_clothing</t>
-  </si>
-  <si>
-    <t>ENG_motorized_focus</t>
-  </si>
-  <si>
-    <t>ENG_tank_focus</t>
-  </si>
-  <si>
-    <t>ENG_cruiser_tanks</t>
-  </si>
-  <si>
-    <t>ENG_bouncing_bomb</t>
-  </si>
-  <si>
-    <t>ENG_support_france</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -436,7 +439,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -444,7 +448,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5168CB-632A-4645-9810-F038E7CD2226}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +824,7 @@
       <c r="B4">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <f>B1+B4</f>
         <v>13164</v>
       </c>
@@ -832,7 +836,7 @@
       <c r="B5">
         <v>28</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <f>B5+C4</f>
         <v>13192</v>
       </c>
@@ -844,7 +848,7 @@
       <c r="B6">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <f t="shared" ref="C6:C13" si="0">B6+C5</f>
         <v>13206</v>
       </c>
@@ -856,7 +860,7 @@
       <c r="B7">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <f t="shared" si="0"/>
         <v>13220</v>
       </c>
@@ -868,7 +872,7 @@
       <c r="B8">
         <v>21</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <f t="shared" si="0"/>
         <v>13241</v>
       </c>
@@ -880,7 +884,7 @@
       <c r="B9">
         <v>21</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <f t="shared" si="0"/>
         <v>13262</v>
       </c>
@@ -892,7 +896,7 @@
       <c r="B10">
         <v>21</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>13283</v>
       </c>
@@ -904,7 +908,7 @@
       <c r="B11">
         <v>14</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="5">
         <f t="shared" si="0"/>
         <v>13297</v>
       </c>
@@ -916,7 +920,7 @@
       <c r="B12">
         <v>28</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <f t="shared" si="0"/>
         <v>13325</v>
       </c>
@@ -928,7 +932,7 @@
       <c r="B13">
         <v>21</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="5">
         <f t="shared" si="0"/>
         <v>13346</v>
       </c>
@@ -940,7 +944,7 @@
       <c r="B14">
         <v>21</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <f t="shared" ref="C14:C45" si="1">B14+C13</f>
         <v>13367</v>
       </c>
@@ -952,7 +956,7 @@
       <c r="B15">
         <v>21</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <f t="shared" si="1"/>
         <v>13388</v>
       </c>
@@ -964,7 +968,7 @@
       <c r="B16">
         <v>21</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="5">
         <f t="shared" si="1"/>
         <v>13409</v>
       </c>
@@ -976,7 +980,7 @@
       <c r="B17">
         <v>14</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="5">
         <f t="shared" si="1"/>
         <v>13423</v>
       </c>
@@ -988,7 +992,7 @@
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="5">
         <f t="shared" si="1"/>
         <v>13437</v>
       </c>
@@ -1000,7 +1004,7 @@
       <c r="B19">
         <v>28</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="5">
         <f t="shared" si="1"/>
         <v>13465</v>
       </c>
@@ -1012,19 +1016,19 @@
       <c r="B20">
         <v>28</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="5">
         <f t="shared" si="1"/>
         <v>13493</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>28</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="5">
         <f t="shared" si="1"/>
         <v>13521</v>
       </c>
@@ -1036,7 +1040,7 @@
       <c r="B22" s="4">
         <v>28</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <f t="shared" si="1"/>
         <v>13549</v>
       </c>
@@ -1049,7 +1053,7 @@
       <c r="B23">
         <v>14</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="5">
         <f t="shared" si="1"/>
         <v>13563</v>
       </c>
@@ -1061,7 +1065,7 @@
       <c r="B24">
         <v>14</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="5">
         <f t="shared" si="1"/>
         <v>13577</v>
       </c>
@@ -1073,7 +1077,7 @@
       <c r="B25">
         <v>28</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="5">
         <f t="shared" si="1"/>
         <v>13605</v>
       </c>
@@ -1085,19 +1089,19 @@
       <c r="B26">
         <v>28</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="5">
         <f t="shared" si="1"/>
         <v>13633</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>28</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="5">
         <f t="shared" si="1"/>
         <v>13661</v>
       </c>
@@ -1109,7 +1113,7 @@
       <c r="B28">
         <v>14</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="5">
         <f t="shared" si="1"/>
         <v>13675</v>
       </c>
@@ -1121,7 +1125,7 @@
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="5">
         <f t="shared" si="1"/>
         <v>13703</v>
       </c>
@@ -1133,7 +1137,7 @@
       <c r="B30">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="5">
         <f t="shared" si="1"/>
         <v>13731</v>
       </c>
@@ -1145,7 +1149,7 @@
       <c r="B31">
         <v>21</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="5">
         <f t="shared" si="1"/>
         <v>13752</v>
       </c>
@@ -1157,43 +1161,43 @@
       <c r="B32">
         <v>28</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="5">
         <f t="shared" si="1"/>
         <v>13780</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33">
         <v>28</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="5">
         <f t="shared" si="1"/>
         <v>13808</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B34">
         <v>28</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="5">
         <f t="shared" si="1"/>
         <v>13836</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35">
         <v>28</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="5">
         <f t="shared" si="1"/>
         <v>13864</v>
       </c>
@@ -1205,7 +1209,7 @@
       <c r="B36">
         <v>28</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="5">
         <f t="shared" si="1"/>
         <v>13892</v>
       </c>
@@ -1217,19 +1221,19 @@
       <c r="B37">
         <v>28</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="5">
         <f t="shared" si="1"/>
         <v>13920</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38">
         <v>28</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="5">
         <f t="shared" si="1"/>
         <v>13948</v>
       </c>
@@ -1241,7 +1245,7 @@
       <c r="B39">
         <v>28</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="5">
         <f t="shared" si="1"/>
         <v>13976</v>
       </c>
@@ -1253,7 +1257,7 @@
       <c r="B40">
         <v>14</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="5">
         <f t="shared" si="1"/>
         <v>13990</v>
       </c>
@@ -1265,7 +1269,7 @@
       <c r="B41">
         <v>28</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="5">
         <f t="shared" si="1"/>
         <v>14018</v>
       </c>
@@ -1277,43 +1281,43 @@
       <c r="B42">
         <v>21</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="5">
         <f t="shared" si="1"/>
         <v>14039</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B43">
         <v>28</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="5">
         <f t="shared" si="1"/>
         <v>14067</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B44">
         <v>28</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="5">
         <f t="shared" si="1"/>
         <v>14095</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45">
         <v>28</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="5">
         <f t="shared" si="1"/>
         <v>14123</v>
       </c>
@@ -1325,8 +1329,8 @@
       <c r="B46">
         <v>28</v>
       </c>
-      <c r="C46" s="1">
-        <f t="shared" ref="C46:C77" si="2">B46+C45</f>
+      <c r="C46" s="5">
+        <f t="shared" ref="C46:C66" si="2">B46+C45</f>
         <v>14151</v>
       </c>
     </row>
@@ -1337,723 +1341,724 @@
       <c r="B47">
         <v>28</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="5">
         <f t="shared" si="2"/>
         <v>14179</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48">
         <v>42</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="5">
         <f t="shared" si="2"/>
         <v>14221</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49">
         <v>28</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="5">
         <f t="shared" si="2"/>
         <v>14249</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50">
         <v>28</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="5">
         <f t="shared" si="2"/>
         <v>14277</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51">
         <v>28</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="5">
         <f t="shared" si="2"/>
         <v>14305</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="B52">
         <v>21</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="5">
         <f t="shared" si="2"/>
         <v>14326</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>28</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="5">
         <f t="shared" si="2"/>
         <v>14354</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54">
         <v>21</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="5">
         <f t="shared" si="2"/>
         <v>14375</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>17</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="5">
         <f t="shared" si="2"/>
         <v>14392</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B56">
         <v>70</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="5">
         <f t="shared" si="2"/>
         <v>14462</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="B57">
         <v>21</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="5">
         <f t="shared" si="2"/>
         <v>14483</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>7</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="5">
         <f t="shared" si="2"/>
         <v>14490</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="B59">
         <v>7</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="5">
         <f t="shared" si="2"/>
         <v>14497</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>14</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="5">
         <f t="shared" si="2"/>
         <v>14511</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>28</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="5">
         <f t="shared" si="2"/>
         <v>14539</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>28</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="5">
         <f t="shared" si="2"/>
         <v>14567</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>14</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="5">
         <f t="shared" si="2"/>
         <v>14581</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>14</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="5">
         <f t="shared" si="2"/>
         <v>14595</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>21</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="5">
         <f t="shared" si="2"/>
         <v>14616</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>28</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="5">
         <f t="shared" si="2"/>
         <v>14644</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>28</v>
       </c>
-      <c r="C67" s="1">
-        <f>B67+C66</f>
+      <c r="C67" s="5">
+        <f t="shared" ref="C67:C106" si="3">B67+C66</f>
         <v>14672</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>28</v>
       </c>
-      <c r="C68" s="1">
-        <f>B68+C67</f>
+      <c r="C68" s="5">
+        <f t="shared" si="3"/>
         <v>14700</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>21</v>
       </c>
-      <c r="C69" s="1">
-        <f>B69+C68</f>
+      <c r="C69" s="5">
+        <f t="shared" si="3"/>
         <v>14721</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>28</v>
       </c>
-      <c r="C70" s="1">
-        <f>B70+C69</f>
+      <c r="C70" s="5">
+        <f t="shared" si="3"/>
         <v>14749</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>28</v>
       </c>
-      <c r="C71" s="1">
-        <f>B71+C70</f>
+      <c r="C71" s="5">
+        <f t="shared" si="3"/>
         <v>14777</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>28</v>
       </c>
-      <c r="C72" s="1">
-        <f>B72+C71</f>
+      <c r="C72" s="5">
+        <f t="shared" si="3"/>
         <v>14805</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>28</v>
       </c>
-      <c r="C73" s="1">
-        <f>B73+C72</f>
+      <c r="C73" s="5">
+        <f t="shared" si="3"/>
         <v>14833</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B74">
         <v>21</v>
       </c>
-      <c r="C74" s="1">
-        <f>B74+C73</f>
+      <c r="C74" s="5">
+        <f t="shared" si="3"/>
         <v>14854</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="B75">
         <v>21</v>
       </c>
-      <c r="C75" s="1">
-        <f>B75+C74</f>
+      <c r="C75" s="5">
+        <f t="shared" si="3"/>
         <v>14875</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="B76">
         <v>21</v>
       </c>
-      <c r="C76" s="1">
-        <f>B76+C75</f>
+      <c r="C76" s="5">
+        <f t="shared" si="3"/>
         <v>14896</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B77">
         <v>28</v>
       </c>
-      <c r="C77" s="1">
-        <f>B77+C76</f>
+      <c r="C77" s="5">
+        <f t="shared" si="3"/>
         <v>14924</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B78">
         <v>28</v>
       </c>
-      <c r="C78" s="1">
-        <f>B78+C77</f>
+      <c r="C78" s="5">
+        <f t="shared" si="3"/>
         <v>14952</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B79">
         <v>28</v>
       </c>
-      <c r="C79" s="1">
-        <f>B79+C78</f>
+      <c r="C79" s="5">
+        <f t="shared" si="3"/>
         <v>14980</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B80">
         <v>28</v>
       </c>
-      <c r="C80" s="1">
-        <f>B80+C79</f>
+      <c r="C80" s="5">
+        <f t="shared" si="3"/>
         <v>15008</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B81">
         <v>7</v>
       </c>
-      <c r="C81" s="1">
-        <f>B81+C80</f>
+      <c r="C81" s="5">
+        <f t="shared" si="3"/>
         <v>15015</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B82">
         <v>28</v>
       </c>
-      <c r="C82" s="1">
-        <f>B82+C81</f>
+      <c r="C82" s="5">
+        <f t="shared" si="3"/>
         <v>15043</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B83">
         <v>28</v>
       </c>
-      <c r="C83" s="1">
-        <f>B83+C82</f>
+      <c r="C83" s="5">
+        <f t="shared" si="3"/>
         <v>15071</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B84">
         <v>28</v>
       </c>
-      <c r="C84" s="1">
-        <f>B84+C83</f>
+      <c r="C84" s="5">
+        <f t="shared" si="3"/>
         <v>15099</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B85">
         <v>28</v>
       </c>
-      <c r="C85" s="1">
-        <f>B85+C84</f>
+      <c r="C85" s="5">
+        <f t="shared" si="3"/>
         <v>15127</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B86">
         <v>28</v>
       </c>
-      <c r="C86" s="1">
-        <f>B86+C85</f>
+      <c r="C86" s="5">
+        <f t="shared" si="3"/>
         <v>15155</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B87">
         <v>28</v>
       </c>
-      <c r="C87" s="1">
-        <f>B87+C86</f>
+      <c r="C87" s="5">
+        <f t="shared" si="3"/>
         <v>15183</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B88">
         <v>28</v>
       </c>
-      <c r="C88" s="1">
-        <f>B88+C87</f>
+      <c r="C88" s="5">
+        <f t="shared" si="3"/>
         <v>15211</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B89">
         <v>28</v>
       </c>
-      <c r="C89" s="1">
-        <f>B89+C88</f>
+      <c r="C89" s="5">
+        <f t="shared" si="3"/>
         <v>15239</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>28</v>
       </c>
-      <c r="C90" s="1">
-        <f>B90+C89</f>
+      <c r="C90" s="5">
+        <f t="shared" si="3"/>
         <v>15267</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>28</v>
       </c>
-      <c r="C91" s="1">
-        <f>B91+C90</f>
+      <c r="C91" s="5">
+        <f t="shared" si="3"/>
         <v>15295</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>28</v>
       </c>
-      <c r="C92" s="1">
-        <f>B92+C91</f>
+      <c r="C92" s="5">
+        <f t="shared" si="3"/>
         <v>15323</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>28</v>
       </c>
-      <c r="C93" s="1">
-        <f>B93+C92</f>
+      <c r="C93" s="5">
+        <f t="shared" si="3"/>
         <v>15351</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>28</v>
       </c>
-      <c r="C94" s="1">
-        <f>B94+C93</f>
+      <c r="C94" s="5">
+        <f t="shared" si="3"/>
         <v>15379</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B95">
         <v>28</v>
       </c>
-      <c r="C95" s="1">
-        <f>B95+C94</f>
+      <c r="C95" s="5">
+        <f t="shared" si="3"/>
         <v>15407</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B96">
         <v>28</v>
       </c>
-      <c r="C96" s="1">
-        <f>B96+C95</f>
+      <c r="C96" s="5">
+        <f t="shared" si="3"/>
         <v>15435</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B97">
         <v>28</v>
       </c>
-      <c r="C97" s="1">
-        <f>B97+C96</f>
+      <c r="C97" s="5">
+        <f t="shared" si="3"/>
         <v>15463</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B98">
         <v>28</v>
       </c>
-      <c r="C98" s="1">
-        <f>B98+C97</f>
+      <c r="C98" s="5">
+        <f t="shared" si="3"/>
         <v>15491</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B99">
         <v>28</v>
       </c>
-      <c r="C99" s="1">
-        <f>B99+C98</f>
+      <c r="C99" s="5">
+        <f t="shared" si="3"/>
         <v>15519</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B100">
         <v>28</v>
       </c>
-      <c r="C100" s="1">
-        <f>B100+C99</f>
+      <c r="C100" s="5">
+        <f t="shared" si="3"/>
         <v>15547</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B101">
         <v>28</v>
       </c>
-      <c r="C101" s="1">
-        <f>B101+C100</f>
+      <c r="C101" s="5">
+        <f t="shared" si="3"/>
         <v>15575</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B102">
         <v>28</v>
       </c>
-      <c r="C102" s="1">
-        <f>B102+C101</f>
+      <c r="C102" s="5">
+        <f t="shared" si="3"/>
         <v>15603</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B103">
         <v>28</v>
       </c>
-      <c r="C103" s="1">
-        <f>B103+C102</f>
+      <c r="C103" s="5">
+        <f t="shared" si="3"/>
         <v>15631</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B104">
         <v>28</v>
       </c>
-      <c r="C104" s="1">
-        <f>B104+C103</f>
+      <c r="C104" s="5">
+        <f t="shared" si="3"/>
         <v>15659</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B105">
         <v>28</v>
       </c>
-      <c r="C105" s="1">
-        <f>B105+C104</f>
+      <c r="C105" s="5">
+        <f t="shared" si="3"/>
         <v>15687</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B106">
         <v>28</v>
       </c>
-      <c r="C106" s="1">
-        <f>B106+C105</f>
+      <c r="C106" s="5">
+        <f t="shared" si="3"/>
         <v>15715</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>